<commit_message>
ajuste planilha monitoramento OBM
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Terminologias/OBM/Monitoramento atividades OBM.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Terminologias/OBM/Monitoramento atividades OBM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Monalisa\Documents\GitHub\HSL-IPS\Entregaveis\Entrega_1_RepositorioSemantico\Terminologias\OBM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/HSL-IPS-1/Entregaveis/1.RepositorioSemantico/Terminologias/OBM/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B422B05-F752-0249-B59E-D08807DDDBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="2360" yWindow="760" windowWidth="23040" windowHeight="14140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitoramento diário" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,28 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="39">
   <si>
     <t>Anotar diariamente as 18h</t>
   </si>
@@ -144,11 +156,14 @@
   <si>
     <t>META DIÁRIA</t>
   </si>
+  <si>
+    <t>março 23</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -219,7 +234,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,8 +295,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -428,11 +449,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -441,6 +473,64 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -468,64 +558,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -537,29 +576,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,7 +629,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -984,7 +1032,7 @@
             <c:numRef>
               <c:f>[1]Calculos!$AI$5:$AI$119</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="115"/>
                 <c:pt idx="0">
                   <c:v>154344.1043478261</c:v>
@@ -1995,7 +2043,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="432043000"/>
@@ -2028,7 +2076,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2054,11 +2101,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
+              <a:endParaRPr lang="en-BR"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2086,7 +2133,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="432042672"/>
@@ -2127,7 +2174,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="en-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6252,23 +6299,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:V12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -6286,996 +6332,1098 @@
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7" t="s">
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="10" t="s">
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="13" t="s">
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="15"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="6"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17" t="s">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="E5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="G5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="H5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="I5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="J5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="K5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="L5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="M5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="20" t="s">
+      <c r="N5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="O5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="20" t="s">
+      <c r="P5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="Q5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="20" t="s">
+      <c r="R5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="R5" s="21" t="s">
+      <c r="S5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S5" s="21" t="s">
+      <c r="T5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="T5" s="21" t="s">
+      <c r="U5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="U5" s="21" t="s">
+      <c r="V5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="V5" s="21" t="s">
+      <c r="W5" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="22">
+      <c r="C6" s="13">
         <v>8</v>
       </c>
-      <c r="C6" s="23">
+      <c r="D6" s="14">
         <v>4561</v>
       </c>
-      <c r="D6" s="24">
+      <c r="E6" s="15">
         <v>3434</v>
       </c>
-      <c r="E6" s="23">
+      <c r="F6" s="14">
         <v>0</v>
       </c>
-      <c r="F6" s="24">
+      <c r="G6" s="15">
         <v>1627</v>
       </c>
-      <c r="G6" s="23">
+      <c r="H6" s="14">
         <v>0</v>
       </c>
-      <c r="H6" s="25">
+      <c r="I6" s="16">
         <v>13197</v>
       </c>
-      <c r="I6" s="25">
+      <c r="J6" s="16">
         <v>11606</v>
       </c>
-      <c r="J6" s="25">
+      <c r="K6" s="16">
         <v>0</v>
       </c>
-      <c r="K6" s="25">
+      <c r="L6" s="16">
         <v>11</v>
       </c>
-      <c r="L6" s="25">
+      <c r="M6" s="16">
         <v>0</v>
       </c>
-      <c r="M6" s="26">
+      <c r="N6" s="17">
         <v>6173</v>
       </c>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26">
+      <c r="O6" s="17"/>
+      <c r="P6" s="17">
         <v>0</v>
       </c>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26">
-        <f>IF(P6&gt;0,P6-#REF!,0)</f>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17">
+        <f>IF(Q6&gt;0,Q6-#REF!,0)</f>
         <v>0</v>
       </c>
-      <c r="R6" s="27">
+      <c r="S6" s="18">
         <v>21313</v>
       </c>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27">
-        <f>IF(S6&gt;0,S6-#REF!,0)</f>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18">
+        <f>IF(T6&gt;0,T6-#REF!,0)</f>
         <v>0</v>
       </c>
-      <c r="U6" s="27"/>
-      <c r="V6" s="27">
-        <f>IF(U6&gt;0,U6-#REF!,0)</f>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18">
+        <f>IF(V6&gt;0,V6-#REF!,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+    <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="65"/>
+      <c r="B7" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="22">
+      <c r="C7" s="13">
         <v>9</v>
       </c>
-      <c r="C7" s="23">
+      <c r="D7" s="14">
         <v>4561</v>
       </c>
-      <c r="D7" s="24">
+      <c r="E7" s="15">
         <v>3535</v>
       </c>
-      <c r="E7" s="23">
-        <f>IF(D7&gt;0,D7-D6,"")</f>
+      <c r="F7" s="14">
+        <f>IF(E7&gt;0,E7-E6,"")</f>
         <v>101</v>
       </c>
-      <c r="F7" s="24">
+      <c r="G7" s="15">
         <v>1642</v>
       </c>
-      <c r="G7" s="23">
-        <f>IF(F7&gt;0,F7-F6,"")</f>
+      <c r="H7" s="14">
+        <f>IF(G7&gt;0,G7-G6,"")</f>
         <v>15</v>
       </c>
-      <c r="H7" s="25">
+      <c r="I7" s="16">
         <v>13197</v>
       </c>
-      <c r="I7" s="25">
+      <c r="J7" s="16">
         <v>11726</v>
       </c>
-      <c r="J7" s="25">
-        <f>IF(I7&gt;0,I7-I6,"")</f>
+      <c r="K7" s="16">
+        <f>IF(J7&gt;0,J7-J6,"")</f>
         <v>120</v>
       </c>
-      <c r="K7" s="25">
+      <c r="L7" s="16">
         <v>11</v>
       </c>
-      <c r="L7" s="25">
-        <f>IF(K7&gt;0,K7-K6,"")</f>
+      <c r="M7" s="16">
+        <f>IF(L7&gt;0,L7-L6,"")</f>
         <v>0</v>
       </c>
-      <c r="M7" s="26">
+      <c r="N7" s="17">
         <v>6173</v>
       </c>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26" t="str">
-        <f>IF(N7&gt;0,N7-N6,"")</f>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17" t="str">
+        <f>IF(O7&gt;0,O7-O6,"")</f>
         <v/>
       </c>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26" t="str">
-        <f>IF(P7&gt;0,P7-P6,"")</f>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17" t="str">
+        <f>IF(Q7&gt;0,Q7-Q6,"")</f>
         <v/>
       </c>
-      <c r="R7" s="27">
+      <c r="S7" s="18">
         <v>21313</v>
       </c>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27" t="str">
-        <f>IF(S7&gt;0,S7-S6,"")</f>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18" t="str">
+        <f>IF(T7&gt;0,T7-T6,"")</f>
         <v/>
       </c>
-      <c r="U7" s="27"/>
-      <c r="V7" s="27" t="str">
-        <f>IF(U7&gt;0,U7-U6,"")</f>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18" t="str">
+        <f>IF(V7&gt;0,V7-V6,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+    <row r="8" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="65"/>
+      <c r="B8" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="22">
+      <c r="C8" s="13">
         <v>10</v>
       </c>
-      <c r="C8" s="23">
+      <c r="D8" s="14">
         <v>4561</v>
       </c>
-      <c r="D8" s="24">
+      <c r="E8" s="15">
         <v>3569</v>
       </c>
-      <c r="E8" s="23">
-        <f t="shared" ref="E8:E12" si="0">IF(D8&gt;0,D8-D7,"")</f>
+      <c r="F8" s="14">
+        <f t="shared" ref="F8:F12" si="0">IF(E8&gt;0,E8-E7,"")</f>
         <v>34</v>
       </c>
-      <c r="F8" s="24">
+      <c r="G8" s="15">
         <v>1708</v>
       </c>
-      <c r="G8" s="23">
-        <f t="shared" ref="G8:G12" si="1">IF(F8&gt;0,F8-F7,"")</f>
+      <c r="H8" s="14">
+        <f t="shared" ref="H8:H12" si="1">IF(G8&gt;0,G8-G7,"")</f>
         <v>66</v>
       </c>
-      <c r="H8" s="25">
+      <c r="I8" s="16">
         <v>13197</v>
       </c>
-      <c r="I8" s="25">
+      <c r="J8" s="16">
         <v>11849</v>
       </c>
-      <c r="J8" s="25">
-        <f t="shared" ref="J8:J12" si="2">IF(I8&gt;0,I8-I7,"")</f>
+      <c r="K8" s="16">
+        <f t="shared" ref="K8:K12" si="2">IF(J8&gt;0,J8-J7,"")</f>
         <v>123</v>
       </c>
-      <c r="K8" s="25">
+      <c r="L8" s="16">
         <v>11</v>
       </c>
-      <c r="L8" s="25">
-        <f t="shared" ref="L8:L12" si="3">IF(K8&gt;0,K8-K7,"")</f>
+      <c r="M8" s="16">
+        <f t="shared" ref="M8:M12" si="3">IF(L8&gt;0,L8-L7,"")</f>
         <v>0</v>
       </c>
-      <c r="M8" s="26">
+      <c r="N8" s="17">
         <v>6173</v>
       </c>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26" t="str">
-        <f t="shared" ref="O8:O12" si="4">IF(N8&gt;0,N8-N7,"")</f>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17" t="str">
+        <f t="shared" ref="P8:P12" si="4">IF(O8&gt;0,O8-O7,"")</f>
         <v/>
       </c>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26" t="str">
-        <f t="shared" ref="Q8:Q12" si="5">IF(P8&gt;0,P8-P7,"")</f>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17" t="str">
+        <f t="shared" ref="R8:R12" si="5">IF(Q8&gt;0,Q8-Q7,"")</f>
         <v/>
       </c>
-      <c r="R8" s="27">
+      <c r="S8" s="18">
         <v>21313</v>
       </c>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27" t="str">
-        <f t="shared" ref="T8:T12" si="6">IF(S8&gt;0,S8-S7,"")</f>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18" t="str">
+        <f t="shared" ref="U8:U12" si="6">IF(T8&gt;0,T8-T7,"")</f>
         <v/>
       </c>
-      <c r="U8" s="27"/>
-      <c r="V8" s="27" t="str">
-        <f t="shared" ref="V8:V12" si="7">IF(U8&gt;0,U8-U7,"")</f>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18" t="str">
+        <f t="shared" ref="W8:W12" si="7">IF(V8&gt;0,V8-V7,"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="65"/>
+      <c r="B9" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="22">
+      <c r="C9" s="13">
         <v>11</v>
       </c>
-      <c r="C9" s="23">
+      <c r="D9" s="14">
         <v>4561</v>
       </c>
-      <c r="D9" s="24">
+      <c r="E9" s="15">
         <v>3616</v>
       </c>
-      <c r="E9" s="23">
+      <c r="F9" s="14">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="F9" s="24">
+      <c r="G9" s="15">
         <v>1769</v>
       </c>
-      <c r="G9" s="23">
+      <c r="H9" s="14">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="H9" s="25">
+      <c r="I9" s="16">
         <v>13197</v>
       </c>
-      <c r="I9" s="25">
+      <c r="J9" s="16">
         <v>12007</v>
       </c>
-      <c r="J9" s="25">
+      <c r="K9" s="16">
         <f t="shared" si="2"/>
         <v>158</v>
       </c>
-      <c r="K9" s="25">
+      <c r="L9" s="16">
         <v>11</v>
       </c>
-      <c r="L9" s="25">
+      <c r="M9" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M9" s="26">
+      <c r="N9" s="17">
         <v>6173</v>
       </c>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26" t="str">
+      <c r="O9" s="17"/>
+      <c r="P9" s="17" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26" t="str">
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="R9" s="27">
+      <c r="S9" s="18">
         <v>21313</v>
       </c>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27" t="str">
+      <c r="T9" s="18"/>
+      <c r="U9" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="U9" s="27"/>
-      <c r="V9" s="27" t="str">
+      <c r="V9" s="18"/>
+      <c r="W9" s="18" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+    <row r="10" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="65"/>
+      <c r="B10" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="22">
+      <c r="C10" s="13">
         <v>12</v>
       </c>
-      <c r="C10" s="23">
+      <c r="D10" s="14">
         <v>4561</v>
       </c>
-      <c r="D10" s="24">
+      <c r="E10" s="15">
         <v>3616</v>
       </c>
-      <c r="E10" s="23">
+      <c r="F10" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F10" s="24">
+      <c r="G10" s="15">
         <v>1769</v>
       </c>
-      <c r="G10" s="23">
+      <c r="H10" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H10" s="25">
+      <c r="I10" s="16">
         <v>13197</v>
       </c>
-      <c r="I10" s="25">
+      <c r="J10" s="16">
         <v>12007</v>
       </c>
-      <c r="J10" s="25">
+      <c r="K10" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K10" s="25">
+      <c r="L10" s="16">
         <v>11</v>
       </c>
-      <c r="L10" s="25">
+      <c r="M10" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M10" s="26">
+      <c r="N10" s="17">
         <v>6173</v>
       </c>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26" t="str">
+      <c r="O10" s="17"/>
+      <c r="P10" s="17" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26" t="str">
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="R10" s="27">
+      <c r="S10" s="18">
         <v>21313</v>
       </c>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27" t="str">
+      <c r="T10" s="18"/>
+      <c r="U10" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="U10" s="27"/>
-      <c r="V10" s="27" t="str">
+      <c r="V10" s="18"/>
+      <c r="W10" s="18" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="15" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+    <row r="11" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="65"/>
+      <c r="B11" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="22">
+      <c r="C11" s="13">
         <v>13</v>
       </c>
-      <c r="C11" s="23">
+      <c r="D11" s="14">
         <v>4561</v>
       </c>
-      <c r="D11" s="24">
+      <c r="E11" s="15">
         <v>3616</v>
       </c>
-      <c r="E11" s="23">
+      <c r="F11" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" s="24">
+      <c r="G11" s="15">
         <v>1769</v>
       </c>
-      <c r="G11" s="23">
+      <c r="H11" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H11" s="25">
+      <c r="I11" s="16">
         <v>13197</v>
       </c>
-      <c r="I11" s="25">
+      <c r="J11" s="16">
         <v>12007</v>
       </c>
-      <c r="J11" s="25">
+      <c r="K11" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K11" s="25">
+      <c r="L11" s="16">
         <v>11</v>
       </c>
-      <c r="L11" s="25">
+      <c r="M11" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M11" s="26">
+      <c r="N11" s="17">
         <v>6173</v>
       </c>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26" t="str">
+      <c r="O11" s="17"/>
+      <c r="P11" s="17" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26" t="str">
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="R11" s="27">
+      <c r="S11" s="18">
         <v>21313</v>
       </c>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27" t="str">
+      <c r="T11" s="18"/>
+      <c r="U11" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="U11" s="27"/>
-      <c r="V11" s="27" t="str">
+      <c r="V11" s="18"/>
+      <c r="W11" s="18" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="15" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+    <row r="12" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="65"/>
+      <c r="B12" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="22">
+      <c r="C12" s="13">
         <v>14</v>
       </c>
-      <c r="C12" s="23">
+      <c r="D12" s="14">
         <v>4561</v>
       </c>
-      <c r="D12" s="24">
+      <c r="E12" s="15">
         <v>3656</v>
       </c>
-      <c r="E12" s="23">
+      <c r="F12" s="14">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F12" s="24">
+      <c r="G12" s="15">
         <v>1823</v>
       </c>
-      <c r="G12" s="23">
+      <c r="H12" s="14">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="H12" s="25">
+      <c r="I12" s="16">
         <v>13197</v>
       </c>
-      <c r="I12" s="25">
+      <c r="J12" s="16">
         <v>12106</v>
       </c>
-      <c r="J12" s="25">
+      <c r="K12" s="16">
         <f t="shared" si="2"/>
         <v>99</v>
       </c>
-      <c r="K12" s="25">
+      <c r="L12" s="16">
         <v>11</v>
       </c>
-      <c r="L12" s="25">
+      <c r="M12" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M12" s="26">
+      <c r="N12" s="17">
         <v>6173</v>
       </c>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26" t="str">
+      <c r="O12" s="17"/>
+      <c r="P12" s="17" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26" t="str">
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="R12" s="27">
+      <c r="S12" s="18">
         <v>21313</v>
       </c>
-      <c r="S12" s="27"/>
-      <c r="T12" s="27" t="str">
+      <c r="T12" s="18"/>
+      <c r="U12" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="U12" s="27"/>
-      <c r="V12" s="27" t="str">
+      <c r="V12" s="18"/>
+      <c r="W12" s="18" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="65"/>
+      <c r="B13" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="13">
+        <f>C12+1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="65"/>
+      <c r="B14" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="13">
+        <f t="shared" ref="C14:C29" si="8">C13+1</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="65"/>
+      <c r="B15" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="13">
+        <f t="shared" si="8"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="65"/>
+      <c r="B16" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="13">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="65"/>
+      <c r="B17" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="13">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="65"/>
+      <c r="B18" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="13">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="65"/>
+      <c r="B19" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="13">
+        <f t="shared" si="8"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="65"/>
+      <c r="B20" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="13">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="65"/>
+      <c r="B21" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="13">
+        <f t="shared" si="8"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="65"/>
+      <c r="B22" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="13">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="65"/>
+      <c r="B23" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="13">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="65"/>
+      <c r="B24" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="13">
+        <f t="shared" si="8"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="65"/>
+      <c r="B25" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="13">
+        <f t="shared" si="8"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="65"/>
+      <c r="B26" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="13">
+        <f t="shared" si="8"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="65"/>
+      <c r="B27" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="13">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="65"/>
+      <c r="B28" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="13">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="65"/>
+      <c r="B29" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="67">
+        <f t="shared" si="8"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="68"/>
+      <c r="C30" s="69"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B31" s="68"/>
+      <c r="C31" s="69"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B32" s="68"/>
+      <c r="C32" s="69"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="M4:Q4"/>
+  <mergeCells count="4">
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="A6:A29"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32" t="s">
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="33" t="s">
+      <c r="I4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="33" t="s">
+      <c r="J4" s="20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="21">
         <v>5</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="21">
         <v>4825</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="21">
         <f>C5*B5</f>
         <v>24125</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="14">
         <v>4824</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="21">
         <f>E5*B5</f>
         <v>24120</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="22">
         <f>(F5*100)/D5</f>
         <v>99.979274611398964</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="21">
         <v>3732</v>
       </c>
-      <c r="I5" s="34">
+      <c r="I5" s="21">
         <f>H5*B5</f>
         <v>18660</v>
       </c>
-      <c r="J5" s="35">
+      <c r="J5" s="22">
         <f>(I5*100)/D5</f>
         <v>77.347150259067362</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="23">
         <v>4</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="23">
         <v>12396</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="23">
         <f t="shared" ref="D6:D8" si="0">C6*B6</f>
         <v>49584</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="16">
         <v>12395</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="23">
         <f>E6*B6</f>
         <v>49580</v>
       </c>
-      <c r="G6" s="37">
+      <c r="G6" s="24">
         <f>(F6*100)/D6</f>
         <v>99.991932881574698</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="16">
         <v>4234</v>
       </c>
-      <c r="I6" s="36">
+      <c r="I6" s="23">
         <f>H6*B6</f>
         <v>16936</v>
       </c>
-      <c r="J6" s="37">
+      <c r="J6" s="24">
         <f t="shared" ref="J6:J9" si="1">(I6*100)/D6</f>
         <v>34.156179412713776</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="38">
+      <c r="B7" s="25">
         <v>1.5</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="25">
         <v>21313</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="25">
         <f t="shared" si="0"/>
         <v>31969.5</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="26">
         <v>600</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="25">
         <f>E7*B7</f>
         <v>900</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="27">
         <f>(F7*100)/D7</f>
         <v>2.8151832215079997</v>
       </c>
-      <c r="H7" s="39">
+      <c r="H7" s="26">
         <v>0</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="25">
         <f t="shared" ref="I7:I8" si="2">H7*B7</f>
         <v>0</v>
       </c>
-      <c r="J7" s="38">
+      <c r="J7" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="41">
+      <c r="B8" s="28">
         <v>1</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="28">
         <v>8721</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="28">
         <f t="shared" si="0"/>
         <v>8721</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="29">
         <v>8720</v>
       </c>
-      <c r="F8" s="41">
+      <c r="F8" s="28">
         <v>990</v>
       </c>
-      <c r="G8" s="43">
+      <c r="G8" s="30">
         <f>(F8*100)/D8</f>
         <v>11.351909184726523</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="29">
         <v>0</v>
       </c>
-      <c r="I8" s="41">
+      <c r="I8" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J8" s="41">
+      <c r="J8" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20">
         <f>C5+C6+C7+C8</f>
         <v>47255</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="20">
         <f>D5+D6+D7+D8</f>
         <v>114399.5</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="20">
         <f>E5+E6+E7+E8</f>
         <v>26539</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="20">
         <f>F5+F6+F7+F8</f>
         <v>75590</v>
       </c>
-      <c r="G9" s="44">
+      <c r="G9" s="31">
         <f>(F9*100)/D9</f>
         <v>66.07546361653678</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="20">
         <f>H5+H6+H7+H8</f>
         <v>7966</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="20">
         <f>I5+I6+I7+I8</f>
         <v>35596</v>
       </c>
-      <c r="J9" s="44">
+      <c r="J9" s="31">
         <f t="shared" si="1"/>
         <v>31.115520609792874</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="45"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D10">
         <f>D9*2</f>
         <v>228799</v>
       </c>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="45"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
+    <row r="12" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="B12" s="32"/>
+      <c r="C12" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="45"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-    </row>
-    <row r="13" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="45"/>
-      <c r="B13" s="47" t="s">
+    <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="B13" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="32">
         <f>C9*2</f>
         <v>94510</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="32">
         <f>D9*2</f>
         <v>228799</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
     </row>
-    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="45"/>
-      <c r="B14" s="47" t="s">
+    <row r="14" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="B14" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C14" s="32">
         <f>E9+H9</f>
         <v>34505</v>
       </c>
-      <c r="D14" s="47">
+      <c r="D14" s="32">
         <f>F9+I9</f>
         <v>111186</v>
       </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
     </row>
-    <row r="15" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="45"/>
-      <c r="B15" s="47" t="s">
+    <row r="15" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="B15" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="48">
+      <c r="C15" s="33">
         <f>(C14*100)/C13</f>
         <v>36.509364088456245</v>
       </c>
-      <c r="D15" s="49">
+      <c r="D15" s="34">
         <f>(D14*100)/D13</f>
         <v>48.595492113164831</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="45"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="45"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="45" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7288,169 +7436,169 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="G3:R14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="15" max="18" width="12.109375" customWidth="1"/>
+    <col min="15" max="18" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="G3" s="50" t="s">
+    <row r="3" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="G3" s="35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="N4" s="51" t="s">
+    <row r="4" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="N4" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="52"/>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="52"/>
-      <c r="R4" s="53"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="58"/>
     </row>
-    <row r="5" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="N5" s="54"/>
-      <c r="O5" s="54" t="s">
+    <row r="5" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="N5" s="36"/>
+      <c r="O5" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54" t="s">
+      <c r="P5" s="36"/>
+      <c r="Q5" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="R5" s="54"/>
+      <c r="R5" s="36"/>
     </row>
-    <row r="6" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="O6" s="55" t="s">
+    <row r="6" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="O6" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="55" t="s">
+      <c r="P6" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="55" t="s">
+      <c r="Q6" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="R6" s="55" t="s">
+      <c r="R6" s="37" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="N7" s="56" t="s">
+    <row r="7" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="N7" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="O7" s="57">
+      <c r="O7" s="39">
         <f>AVERAGE([1]Calculos!F5:F119)</f>
         <v>12.095652173913043</v>
       </c>
-      <c r="P7" s="57">
+      <c r="P7" s="39">
         <f>AVERAGE([1]Calculos!I5:I119)</f>
         <v>18.304347826086957</v>
       </c>
-      <c r="Q7" s="57">
+      <c r="Q7" s="39">
         <f>[1]Calculos!V119/[1]Calculos!AL119</f>
         <v>0</v>
       </c>
-      <c r="R7" s="57">
+      <c r="R7" s="39">
         <f>[1]Calculos!J119/[1]Calculos!AL119</f>
         <v>24.288888888888888</v>
       </c>
     </row>
-    <row r="8" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="N8" s="58" t="s">
+    <row r="8" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="N8" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="57">
+      <c r="O8" s="39">
         <f>AVERAGE([1]Calculos!M5:M119)</f>
         <v>6.8608695652173912</v>
       </c>
-      <c r="P8" s="57">
+      <c r="P8" s="39">
         <f>AVERAGE([1]Calculos!P5:P119)</f>
         <v>36.721739130434784</v>
       </c>
-      <c r="Q8" s="57">
+      <c r="Q8" s="39">
         <f>[1]Calculos!N119/[1]Calculos!AL119</f>
         <v>2.2222222222222223E-2</v>
       </c>
-      <c r="R8" s="57">
+      <c r="R8" s="39">
         <f>[1]Calculos!Q119/[1]Calculos!AL119</f>
         <v>181.37777777777777</v>
       </c>
     </row>
-    <row r="9" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="N9" s="59" t="s">
+    <row r="9" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="N9" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="O9" s="57">
+      <c r="O9" s="39">
         <f>AVERAGE([1]Calculos!AA5:AA119)</f>
         <v>5.2173913043478262</v>
       </c>
-      <c r="P9" s="57">
+      <c r="P9" s="39">
         <f>AVERAGE([1]Calculos!P5:P119)</f>
         <v>36.721739130434784</v>
       </c>
-      <c r="Q9" s="57">
+      <c r="Q9" s="39">
         <f>[1]Calculos!AB119/[1]Calculos!AL119</f>
         <v>473.62222222222221</v>
       </c>
-      <c r="R9" s="57">
+      <c r="R9" s="39">
         <f>[1]Calculos!AE119/[1]Calculos!AL119</f>
         <v>473.62222222222221</v>
       </c>
     </row>
-    <row r="10" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="N10" s="60" t="s">
+    <row r="10" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="N10" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="O10" s="57">
+      <c r="O10" s="39">
         <f>AVERAGE([1]Calculos!T5:T119)</f>
         <v>75.826086956521735</v>
       </c>
-      <c r="P10" s="57">
+      <c r="P10" s="39">
         <f>AVERAGE([1]Calculos!P5:P119)</f>
         <v>36.721739130434784</v>
       </c>
-      <c r="Q10" s="57">
+      <c r="Q10" s="39">
         <f>[1]Calculos!U119/[1]Calculos!AL119</f>
         <v>193.8</v>
       </c>
-      <c r="R10" s="57">
+      <c r="R10" s="39">
         <f>[1]Calculos!X119/[1]Calculos!AL119</f>
         <v>137.17777777777778</v>
       </c>
     </row>
-    <row r="11" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="Q11" s="61" t="s">
+    <row r="11" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="Q11" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="R11" s="62"/>
+      <c r="R11" s="60"/>
     </row>
-    <row r="12" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="Q12" s="63">
+    <row r="12" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="Q12" s="43">
         <f>SUM(Q7:Q10)</f>
         <v>667.44444444444446</v>
       </c>
-      <c r="R12" s="63">
+      <c r="R12" s="43">
         <f>SUM(R7:R10)</f>
         <v>816.4666666666667</v>
       </c>
     </row>
-    <row r="13" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="Q13" s="61" t="s">
+    <row r="13" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="Q13" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="R13" s="62"/>
+      <c r="R13" s="60"/>
     </row>
-    <row r="14" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="Q14" s="64">
+    <row r="14" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="Q14" s="61">
         <f>Q12+R12</f>
         <v>1483.911111111111</v>
       </c>
-      <c r="R14" s="65"/>
+      <c r="R14" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>